<commit_message>
Split power board into its own PCB
</commit_message>
<xml_diff>
--- a/Control Board/control_board_fields.xlsx
+++ b/Control Board/control_board_fields.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="160">
   <si>
     <t>Refs</t>
   </si>
@@ -38,6 +38,9 @@
     <t>668-1018-ND</t>
   </si>
   <si>
+    <t>Buzzers_Beepers:Buzzer_12x9.5RM7.6</t>
+  </si>
+  <si>
     <t>AI-1223-TWT-12V-R</t>
   </si>
   <si>
@@ -56,19 +59,25 @@
     <t>P122625-ND</t>
   </si>
   <si>
+    <t>Capacitors_THT:CP_Radial_D10.0mm_P5.00mm</t>
+  </si>
+  <si>
     <t>470 uF</t>
   </si>
   <si>
-    <t>C9, C10, C14, C15</t>
+    <t>C9</t>
   </si>
   <si>
     <t>445-14423-1-ND</t>
   </si>
   <si>
+    <t>Capacitors_SMD:C_0805</t>
+  </si>
+  <si>
     <t>15 uF</t>
   </si>
   <si>
-    <t>C11, C12, C16, C17, C20, C21</t>
+    <t>C11</t>
   </si>
   <si>
     <t>1276-6526-1-ND</t>
@@ -77,7 +86,7 @@
     <t>22 uF</t>
   </si>
   <si>
-    <t>C8, C13, C18</t>
+    <t>C8</t>
   </si>
   <si>
     <t>399-1171-1-ND</t>
@@ -92,15 +101,21 @@
     <t>445-8046-1-ND</t>
   </si>
   <si>
+    <t>Capacitors_SMD:C_1206</t>
+  </si>
+  <si>
     <t>33 uF</t>
   </si>
   <si>
-    <t>C2-C7, C22-C26, C28-C31, C33, C35, C36, C38, C40, C41, C43, C45, C46, C48, C50, C51, C53, C55, C56</t>
+    <t>C2</t>
   </si>
   <si>
     <t>445-5667-1-ND</t>
   </si>
   <si>
+    <t>Capacitors_SMD:C_0603</t>
+  </si>
+  <si>
     <t>C27</t>
   </si>
   <si>
@@ -110,7 +125,7 @@
     <t>10 uF</t>
   </si>
   <si>
-    <t>C32, C34, C37, C39, C42, C44, C47, C49, C52, C54</t>
+    <t>C32</t>
   </si>
   <si>
     <t>399-1091-1-ND</t>
@@ -119,12 +134,15 @@
     <t>0.01 uF</t>
   </si>
   <si>
-    <t>D1, D3, D4</t>
+    <t>D1</t>
   </si>
   <si>
     <t>SMBJ26CAFSCT-ND</t>
   </si>
   <si>
+    <t>Diodes_SMD:D_SMB</t>
+  </si>
+  <si>
     <t>SMBJ26CA</t>
   </si>
   <si>
@@ -137,12 +155,15 @@
     <t>SMBJ26A</t>
   </si>
   <si>
-    <t>D5, D6</t>
+    <t>D5</t>
   </si>
   <si>
     <t>160-1447-1-ND</t>
   </si>
   <si>
+    <t>LEDs:LED_0603</t>
+  </si>
+  <si>
     <t>LED_R</t>
   </si>
   <si>
@@ -170,6 +191,9 @@
     <t>S9015E-03-ND</t>
   </si>
   <si>
+    <t>Pin_Headers:Pin_Header_Angled_2x03_Pitch1.27mm</t>
+  </si>
+  <si>
     <t>Conn_02x03_Odd_Even</t>
   </si>
   <si>
@@ -179,15 +203,21 @@
     <t>S3324-ND</t>
   </si>
   <si>
+    <t>Custom Footprints:CONN_CARD_02x35_MALE</t>
+  </si>
+  <si>
     <t>Conn_02x35_Counter_Clockwise</t>
   </si>
   <si>
-    <t>L1, L2</t>
+    <t>L1</t>
   </si>
   <si>
     <t>732-3880-1-ND</t>
   </si>
   <si>
+    <t>Inductors_SMD:L_Wuerth_HCI-1365</t>
+  </si>
+  <si>
     <t>18 uH</t>
   </si>
   <si>
@@ -197,6 +227,9 @@
     <t>732-4180-1-ND</t>
   </si>
   <si>
+    <t>Inductors_SMD:L_Wuerth_HCI-1050</t>
+  </si>
+  <si>
     <t>16 uH</t>
   </si>
   <si>
@@ -206,37 +239,49 @@
     <t>490-1174-1-ND</t>
   </si>
   <si>
+    <t>Inductors_SMD:L_0603</t>
+  </si>
+  <si>
     <t>27 nH</t>
   </si>
   <si>
-    <t>Q1-Q6</t>
+    <t>Q1</t>
   </si>
   <si>
     <t>SI7135DP-T1-GE3CT-ND</t>
   </si>
   <si>
+    <t>Custom Footprints:PowerPAK_SO-8</t>
+  </si>
+  <si>
     <t>SI7135DP</t>
   </si>
   <si>
-    <t>Q7, Q8</t>
+    <t>Q7</t>
   </si>
   <si>
     <t>497-3226-1-ND</t>
   </si>
   <si>
+    <t>Housings_SOIC:SOIC-8_3.9x4.9mm_Pitch1.27mm</t>
+  </si>
+  <si>
     <t>STS4DNF60L</t>
   </si>
   <si>
-    <t>R1, R4, R7</t>
+    <t>R1</t>
   </si>
   <si>
     <t>311-93.1KHRCT-ND</t>
   </si>
   <si>
+    <t>Resistors_SMD:R_0603</t>
+  </si>
+  <si>
     <t>93.1 kΩ</t>
   </si>
   <si>
-    <t>R10, R12, R14</t>
+    <t>R10</t>
   </si>
   <si>
     <t>311-100KHRCT-ND</t>
@@ -245,7 +290,7 @@
     <t>100 kΩ</t>
   </si>
   <si>
-    <t>R11, R13</t>
+    <t>R11</t>
   </si>
   <si>
     <t>311-22.0KHRCT-ND</t>
@@ -263,7 +308,7 @@
     <t>6.34 kΩ</t>
   </si>
   <si>
-    <t>R16, R17</t>
+    <t>R16</t>
   </si>
   <si>
     <t>311-1.80KHRCT-ND</t>
@@ -272,7 +317,7 @@
     <t>1.8 kΩ</t>
   </si>
   <si>
-    <t>R18, R19, R28, R31, R32, R34, R36, R38</t>
+    <t>R18</t>
   </si>
   <si>
     <t>311-1.00KHRCT-ND</t>
@@ -290,7 +335,7 @@
     <t>309 Ω</t>
   </si>
   <si>
-    <t>R20-R22</t>
+    <t>R20</t>
   </si>
   <si>
     <t>311-10.0KHRCT-ND</t>
@@ -299,7 +344,7 @@
     <t>10 kΩ</t>
   </si>
   <si>
-    <t>R23-R26</t>
+    <t>R23</t>
   </si>
   <si>
     <t>311-100GRCT-ND</t>
@@ -308,7 +353,7 @@
     <t>100 Ω</t>
   </si>
   <si>
-    <t>R27, R29, R30, R35, R37</t>
+    <t>R27</t>
   </si>
   <si>
     <t>311-20.0KHRCT-ND</t>
@@ -341,7 +386,7 @@
     <t>311-100HRCT-ND</t>
   </si>
   <si>
-    <t>R5, R8</t>
+    <t>R5</t>
   </si>
   <si>
     <t>311-2.49KHRCT-ND</t>
@@ -350,7 +395,7 @@
     <t>2.49 kΩ</t>
   </si>
   <si>
-    <t>R6, R9</t>
+    <t>R6</t>
   </si>
   <si>
     <t>311-5.90KHRCT-ND</t>
@@ -359,12 +404,15 @@
     <t>5.9 kΩ</t>
   </si>
   <si>
-    <t>RN1, RN2</t>
+    <t>RN1</t>
   </si>
   <si>
     <t>MPMT-1K/5KCT-ND</t>
   </si>
   <si>
+    <t>TO_SOT_Packages_SMD:SOT-23</t>
+  </si>
+  <si>
     <t>1 kΩ, 5 kΩ</t>
   </si>
   <si>
@@ -374,6 +422,9 @@
     <t>401-1999-1-ND</t>
   </si>
   <si>
+    <t>Buttons_Switches_SMD:SW_SPDT_CK-JS102011SAQN</t>
+  </si>
+  <si>
     <t>SW_SPDT</t>
   </si>
   <si>
@@ -383,24 +434,33 @@
     <t>LTC4417CGN#PBF-ND</t>
   </si>
   <si>
+    <t>Housings_SSOP:SSOP-24_3.9x8.7mm_Pitch0.635mm</t>
+  </si>
+  <si>
     <t>LTC4417CGN</t>
   </si>
   <si>
-    <t>U9-U13</t>
+    <t>U9</t>
   </si>
   <si>
     <t>MAX31856MUD+-ND</t>
   </si>
   <si>
+    <t>Housings_SSOP:TSSOP-14_4.4x5mm_Pitch0.65mm</t>
+  </si>
+  <si>
     <t>MAX31856</t>
   </si>
   <si>
-    <t>U2-U4</t>
+    <t>U2</t>
   </si>
   <si>
     <t>296-47880-1-ND</t>
   </si>
   <si>
+    <t>TO_SOT_Packages_SMD:SOT-23-6</t>
+  </si>
+  <si>
     <t>TPS54308DDC</t>
   </si>
   <si>
@@ -410,13 +470,19 @@
     <t>ATXMEGA128A3-AU-ND</t>
   </si>
   <si>
+    <t>Housings_QFP:TQFP-64_14x14mm_Pitch0.8mm</t>
+  </si>
+  <si>
     <t>ATXMEGA128A3-AU</t>
   </si>
   <si>
-    <t>U6, U7</t>
+    <t>U6</t>
   </si>
   <si>
     <t>LT1797CS5#TRMPBFCT-ND</t>
+  </si>
+  <si>
+    <t>TO_SOT_Packages_SMD:TSOT-23-5</t>
   </si>
   <si>
     <t>LT1797</t>
@@ -797,581 +863,671 @@
         <v>6</v>
       </c>
       <c r="C2" t="s"/>
-      <c r="D2" t="s"/>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s"/>
-      <c r="D3" t="s"/>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s"/>
-      <c r="D4" t="s"/>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s"/>
-      <c r="D5" t="s"/>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s"/>
+      <c r="D6" t="s">
         <v>18</v>
       </c>
-      <c r="C6" t="s"/>
-      <c r="D6" t="s"/>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s"/>
-      <c r="D7" t="s"/>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
       <c r="E7" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s"/>
-      <c r="D8" t="s"/>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
       <c r="E8" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s"/>
-      <c r="D9" t="s"/>
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
       <c r="E9" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s"/>
-      <c r="D10" t="s"/>
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
       <c r="E10" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" t="s"/>
+      <c r="D11" t="s">
         <v>32</v>
       </c>
-      <c r="C11" t="s"/>
-      <c r="D11" t="s"/>
       <c r="E11" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s"/>
-      <c r="D12" t="s"/>
+      <c r="D12" t="s">
+        <v>41</v>
+      </c>
       <c r="E12" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s"/>
-      <c r="D13" t="s"/>
+      <c r="D13" t="s">
+        <v>41</v>
+      </c>
       <c r="E13" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C14" t="s"/>
-      <c r="D14" t="s"/>
+      <c r="D14" t="s">
+        <v>48</v>
+      </c>
       <c r="E14" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="C15" t="s"/>
-      <c r="D15" t="s"/>
+      <c r="D15" t="s">
+        <v>48</v>
+      </c>
       <c r="E15" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C16" t="s"/>
-      <c r="D16" t="s"/>
+      <c r="D16" t="s">
+        <v>48</v>
+      </c>
       <c r="E16" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="C17" t="s"/>
-      <c r="D17" t="s"/>
+      <c r="D17" t="s">
+        <v>58</v>
+      </c>
       <c r="E17" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="B18" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="C18" t="s"/>
-      <c r="D18" t="s"/>
+      <c r="D18" t="s">
+        <v>62</v>
+      </c>
       <c r="E18" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="B19" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="C19" t="s"/>
-      <c r="D19" t="s"/>
+      <c r="D19" t="s">
+        <v>66</v>
+      </c>
       <c r="E19" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="B20" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C20" t="s"/>
-      <c r="D20" t="s"/>
+      <c r="D20" t="s">
+        <v>70</v>
+      </c>
       <c r="E20" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="B21" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="C21" t="s"/>
-      <c r="D21" t="s"/>
+      <c r="D21" t="s">
+        <v>74</v>
+      </c>
       <c r="E21" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="B22" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="C22" t="s"/>
-      <c r="D22" t="s"/>
+      <c r="D22" t="s">
+        <v>78</v>
+      </c>
       <c r="E22" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="B23" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="C23" t="s"/>
-      <c r="D23" t="s"/>
+      <c r="D23" t="s">
+        <v>82</v>
+      </c>
       <c r="E23" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="B24" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="C24" t="s"/>
-      <c r="D24" t="s"/>
+      <c r="D24" t="s">
+        <v>86</v>
+      </c>
       <c r="E24" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="B25" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
       <c r="C25" t="s"/>
-      <c r="D25" t="s"/>
+      <c r="D25" t="s">
+        <v>86</v>
+      </c>
       <c r="E25" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="B26" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="C26" t="s"/>
-      <c r="D26" t="s"/>
+      <c r="D26" t="s">
+        <v>86</v>
+      </c>
       <c r="E26" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="B27" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="C27" t="s"/>
-      <c r="D27" t="s"/>
+      <c r="D27" t="s">
+        <v>86</v>
+      </c>
       <c r="E27" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="B28" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="C28" t="s"/>
-      <c r="D28" t="s"/>
+      <c r="D28" t="s">
+        <v>86</v>
+      </c>
       <c r="E28" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="B29" t="s">
+        <v>101</v>
+      </c>
+      <c r="C29" t="s"/>
+      <c r="D29" t="s">
         <v>86</v>
       </c>
-      <c r="C29" t="s"/>
-      <c r="D29" t="s"/>
       <c r="E29" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="B30" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="C30" t="s"/>
-      <c r="D30" t="s"/>
+      <c r="D30" t="s">
+        <v>86</v>
+      </c>
       <c r="E30" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="B31" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="C31" t="s"/>
-      <c r="D31" t="s"/>
+      <c r="D31" t="s">
+        <v>86</v>
+      </c>
       <c r="E31" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="B32" t="s">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="C32" t="s"/>
-      <c r="D32" t="s"/>
+      <c r="D32" t="s">
+        <v>86</v>
+      </c>
       <c r="E32" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="B33" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
       <c r="C33" t="s"/>
-      <c r="D33" t="s"/>
+      <c r="D33" t="s">
+        <v>86</v>
+      </c>
       <c r="E33" t="s">
-        <v>99</v>
+        <v>114</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="B34" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="C34" t="s"/>
-      <c r="D34" t="s"/>
+      <c r="D34" t="s">
+        <v>86</v>
+      </c>
       <c r="E34" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="B35" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
       <c r="C35" t="s"/>
-      <c r="D35" t="s"/>
+      <c r="D35" t="s">
+        <v>86</v>
+      </c>
       <c r="E35" t="s">
-        <v>105</v>
+        <v>120</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="B36" t="s">
-        <v>107</v>
+        <v>122</v>
       </c>
       <c r="C36" t="s"/>
-      <c r="D36" t="s"/>
+      <c r="D36" t="s">
+        <v>86</v>
+      </c>
       <c r="E36" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="B37" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="C37" t="s"/>
-      <c r="D37" t="s"/>
+      <c r="D37" t="s">
+        <v>86</v>
+      </c>
       <c r="E37" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
       <c r="B38" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="C38" t="s"/>
-      <c r="D38" t="s"/>
+      <c r="D38" t="s">
+        <v>86</v>
+      </c>
       <c r="E38" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>114</v>
+        <v>129</v>
       </c>
       <c r="B39" t="s">
-        <v>115</v>
+        <v>130</v>
       </c>
       <c r="C39" t="s"/>
-      <c r="D39" t="s"/>
+      <c r="D39" t="s">
+        <v>131</v>
+      </c>
       <c r="E39" t="s">
-        <v>116</v>
+        <v>132</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
       <c r="B40" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="C40" t="s"/>
-      <c r="D40" t="s"/>
+      <c r="D40" t="s">
+        <v>135</v>
+      </c>
       <c r="E40" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
       <c r="B41" t="s">
-        <v>121</v>
+        <v>138</v>
       </c>
       <c r="C41" t="s"/>
-      <c r="D41" t="s"/>
+      <c r="D41" t="s">
+        <v>139</v>
+      </c>
       <c r="E41" t="s">
-        <v>122</v>
+        <v>140</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
       <c r="B42" t="s">
-        <v>124</v>
+        <v>142</v>
       </c>
       <c r="C42" t="s"/>
-      <c r="D42" t="s"/>
+      <c r="D42" t="s">
+        <v>143</v>
+      </c>
       <c r="E42" t="s">
-        <v>125</v>
+        <v>144</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>126</v>
+        <v>145</v>
       </c>
       <c r="B43" t="s">
-        <v>127</v>
+        <v>146</v>
       </c>
       <c r="C43" t="s"/>
-      <c r="D43" t="s"/>
+      <c r="D43" t="s">
+        <v>147</v>
+      </c>
       <c r="E43" t="s">
-        <v>128</v>
+        <v>148</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" t="s">
-        <v>129</v>
+        <v>149</v>
       </c>
       <c r="B44" t="s">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="C44" t="s"/>
-      <c r="D44" t="s"/>
+      <c r="D44" t="s">
+        <v>151</v>
+      </c>
       <c r="E44" t="s">
-        <v>131</v>
+        <v>152</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>132</v>
+        <v>153</v>
       </c>
       <c r="B45" t="s">
-        <v>133</v>
+        <v>154</v>
       </c>
       <c r="C45" t="s"/>
-      <c r="D45" t="s"/>
+      <c r="D45" t="s">
+        <v>155</v>
+      </c>
       <c r="E45" t="s">
-        <v>134</v>
+        <v>156</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>135</v>
+        <v>157</v>
       </c>
       <c r="B46" t="s">
-        <v>136</v>
+        <v>158</v>
       </c>
       <c r="C46" t="s"/>
-      <c r="D46" t="s"/>
+      <c r="D46" t="s">
+        <v>82</v>
+      </c>
       <c r="E46" t="s">
-        <v>137</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>